<commit_message>
second commit with graphs 2-4 made
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophia/Desktop/R Projects/gov-2213/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F5D4A7-C3FB-9744-BE32-7D7DEC23E2E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD01C5E5-922C-C940-8D2A-C6F8091D03DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="680" windowWidth="20960" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="20960" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="80000"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -383,7 +383,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J29"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>